<commit_message>
[New] Data update & launch visualisation with pathway log in *.csv file
</commit_message>
<xml_diff>
--- a/data/methods_graph.xlsx
+++ b/data/methods_graph.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\graph\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antonovae\Desktop\!!Финальные материалы\!!Финальные материалы\База данных\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="950" yWindow="0" windowWidth="28800" windowHeight="13040"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -548,7 +548,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -864,23 +864,23 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.7265625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="22.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28" style="2" customWidth="1"/>
-    <col min="8" max="8" width="25.54296875" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="2"/>
+    <col min="8" max="8" width="25.5703125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -903,7 +903,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -926,7 +926,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -947,7 +947,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -968,7 +968,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -989,7 +989,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -1054,7 +1054,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="3" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" s="3" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -1117,7 +1117,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -1138,7 +1138,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" s="4" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -1161,7 +1161,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" s="4" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -1182,7 +1182,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -1276,7 +1276,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -1321,7 +1321,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="4" customFormat="1" ht="62" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" s="4" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
@@ -1344,7 +1344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>18</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>18</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>18</v>
       </c>
@@ -1430,7 +1430,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="4" customFormat="1" ht="62" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" s="4" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>18</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="4" customFormat="1" ht="62" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" s="4" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>18</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>18</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>18</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>18</v>
       </c>
@@ -1541,7 +1541,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>18</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>18</v>
       </c>
@@ -1585,7 +1585,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>18</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>18</v>
       </c>
@@ -1627,7 +1627,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>18</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>18</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>18</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" s="4" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>23</v>
       </c>
@@ -1713,7 +1713,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:7" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" s="4" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>23</v>
       </c>
@@ -1734,7 +1734,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" s="4" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>23</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:7" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>23</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:7" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>23</v>
       </c>
@@ -1799,7 +1799,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>23</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:7" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>23</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:7" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>23</v>
       </c>
@@ -1862,7 +1862,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:7" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>23</v>
       </c>
@@ -1883,7 +1883,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:7" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>23</v>
       </c>
@@ -1906,7 +1906,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:7" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" s="4" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>23</v>
       </c>
@@ -1927,7 +1927,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:7" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>23</v>
       </c>
@@ -1948,7 +1948,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:7" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>23</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:7" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>23</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:7" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>23</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:7" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>23</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:7" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>23</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:7" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" s="4" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>23</v>
       </c>
@@ -2076,7 +2076,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:7" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>23</v>
       </c>
@@ -2097,7 +2097,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:7" s="4" customFormat="1" ht="62" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" s="4" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>23</v>
       </c>
@@ -2118,7 +2118,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:7" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>23</v>
       </c>
@@ -2141,7 +2141,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:7" s="4" customFormat="1" ht="62" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" s="4" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>23</v>
       </c>
@@ -2162,7 +2162,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:7" s="4" customFormat="1" ht="62" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" s="4" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>23</v>
       </c>
@@ -2183,7 +2183,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:7" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>23</v>
       </c>
@@ -2204,7 +2204,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:7" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>32</v>
       </c>
@@ -2227,7 +2227,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:7" s="4" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" s="4" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>32</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:7" s="4" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" s="4" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>32</v>
       </c>
@@ -2269,7 +2269,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:7" s="4" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" s="4" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>32</v>
       </c>
@@ -2292,7 +2292,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:7" s="4" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" s="4" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>32</v>
       </c>
@@ -2313,7 +2313,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:7" s="4" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" s="4" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>32</v>
       </c>
@@ -2336,7 +2336,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:7" s="4" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" s="4" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>32</v>
       </c>
@@ -2357,7 +2357,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:7" s="4" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" s="4" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>32</v>
       </c>
@@ -2378,7 +2378,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:7" s="4" customFormat="1" ht="62" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" s="4" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>32</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:7" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>32</v>
       </c>
@@ -2422,7 +2422,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:7" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>32</v>
       </c>
@@ -2443,84 +2443,84 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:7" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="74" spans="1:7" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="75" spans="1:7" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="76" spans="1:7" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="77" spans="1:7" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="78" spans="1:7" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="79" spans="1:7" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="80" spans="1:7" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="81" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="82" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="83" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="84" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="85" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="86" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="87" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="98" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="99" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="100" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="101" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="102" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="103" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="104" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="105" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="106" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="107" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="108" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="109" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="110" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="111" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="112" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="113" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="114" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="115" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="116" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="117" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="118" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="119" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="120" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="121" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="122" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="123" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="124" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="125" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="126" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="127" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="128" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="129" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="130" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="131" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="132" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="133" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="134" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="135" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="136" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="137" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="138" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="139" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="140" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="141" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="142" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="143" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="144" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="145" spans="1:6" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="146" spans="1:6" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="147" spans="1:6" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="148" spans="1:6" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="149" spans="1:6" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="150" spans="1:6" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="151" spans="1:6" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="152" spans="1:6" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="153" spans="1:6" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="154" spans="1:6" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="155" spans="1:6" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="156" spans="1:6" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="157" spans="1:6" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="158" spans="1:6" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="159" spans="1:6" s="4" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="160" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="1:7" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="1:7" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="1:7" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="1:7" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="1:7" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="1:7" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="1:7" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="81" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="82" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="83" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="84" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="85" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="86" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="87" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="98" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="99" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="100" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="101" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="102" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="103" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="104" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="105" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="106" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="107" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="108" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="109" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="110" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="111" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="112" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="113" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="114" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="115" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="116" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="117" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="118" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="119" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="120" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="121" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="122" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="123" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="124" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="125" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="126" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="127" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="128" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="129" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="130" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="131" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="132" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="133" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="134" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="135" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="136" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="137" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="138" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="139" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="140" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="141" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="142" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="143" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="144" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="145" spans="1:6" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="146" spans="1:6" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="147" spans="1:6" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="148" spans="1:6" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="149" spans="1:6" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="150" spans="1:6" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="151" spans="1:6" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="152" spans="1:6" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="153" spans="1:6" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="154" spans="1:6" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="155" spans="1:6" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="156" spans="1:6" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="157" spans="1:6" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="158" spans="1:6" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="159" spans="1:6" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="160" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A160" s="2"/>
       <c r="B160" s="2"/>
       <c r="C160" s="2"/>
@@ -2528,7 +2528,7 @@
       <c r="E160" s="2"/>
       <c r="F160" s="2"/>
     </row>
-    <row r="161" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A161" s="2"/>
       <c r="B161" s="2"/>
       <c r="C161" s="2"/>
@@ -2536,7 +2536,7 @@
       <c r="E161" s="2"/>
       <c r="F161" s="2"/>
     </row>
-    <row r="162" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A162" s="2"/>
       <c r="B162" s="2"/>
       <c r="C162" s="2"/>
@@ -2544,7 +2544,7 @@
       <c r="E162" s="2"/>
       <c r="F162" s="2"/>
     </row>
-    <row r="163" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A163" s="2"/>
       <c r="B163" s="2"/>
       <c r="C163" s="2"/>
@@ -2552,7 +2552,7 @@
       <c r="E163" s="2"/>
       <c r="F163" s="2"/>
     </row>
-    <row r="164" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A164" s="2"/>
       <c r="B164" s="2"/>
       <c r="C164" s="2"/>
@@ -2560,7 +2560,7 @@
       <c r="E164" s="2"/>
       <c r="F164" s="2"/>
     </row>
-    <row r="165" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A165" s="2"/>
       <c r="B165" s="2"/>
       <c r="C165" s="2"/>
@@ -2568,7 +2568,7 @@
       <c r="E165" s="2"/>
       <c r="F165" s="2"/>
     </row>
-    <row r="166" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A166" s="2"/>
       <c r="B166" s="2"/>
       <c r="C166" s="2"/>
@@ -2576,7 +2576,7 @@
       <c r="E166" s="2"/>
       <c r="F166" s="2"/>
     </row>
-    <row r="167" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A167" s="2"/>
       <c r="B167" s="2"/>
       <c r="C167" s="2"/>
@@ -2584,7 +2584,7 @@
       <c r="E167" s="2"/>
       <c r="F167" s="2"/>
     </row>
-    <row r="168" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A168" s="2"/>
       <c r="B168" s="2"/>
       <c r="C168" s="2"/>
@@ -2592,7 +2592,7 @@
       <c r="E168" s="2"/>
       <c r="F168" s="2"/>
     </row>
-    <row r="169" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A169" s="2"/>
       <c r="B169" s="2"/>
       <c r="C169" s="2"/>
@@ -2600,7 +2600,7 @@
       <c r="E169" s="2"/>
       <c r="F169" s="2"/>
     </row>
-    <row r="170" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A170" s="2"/>
       <c r="B170" s="2"/>
       <c r="C170" s="2"/>
@@ -2608,7 +2608,7 @@
       <c r="E170" s="2"/>
       <c r="F170" s="2"/>
     </row>
-    <row r="171" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A171" s="2"/>
       <c r="B171" s="2"/>
       <c r="C171" s="2"/>
@@ -2616,7 +2616,7 @@
       <c r="E171" s="2"/>
       <c r="F171" s="2"/>
     </row>
-    <row r="172" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A172" s="2"/>
       <c r="B172" s="2"/>
       <c r="C172" s="2"/>
@@ -2624,7 +2624,7 @@
       <c r="E172" s="2"/>
       <c r="F172" s="2"/>
     </row>
-    <row r="173" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A173" s="2"/>
       <c r="B173" s="2"/>
       <c r="C173" s="2"/>
@@ -2632,7 +2632,7 @@
       <c r="E173" s="2"/>
       <c r="F173" s="2"/>
     </row>
-    <row r="174" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A174" s="2"/>
       <c r="B174" s="2"/>
       <c r="C174" s="2"/>
@@ -2640,7 +2640,7 @@
       <c r="E174" s="2"/>
       <c r="F174" s="2"/>
     </row>
-    <row r="175" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A175" s="2"/>
       <c r="B175" s="2"/>
       <c r="C175" s="2"/>
@@ -2648,7 +2648,7 @@
       <c r="E175" s="2"/>
       <c r="F175" s="2"/>
     </row>
-    <row r="176" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A176" s="2"/>
       <c r="B176" s="2"/>
       <c r="C176" s="2"/>
@@ -2656,7 +2656,7 @@
       <c r="E176" s="2"/>
       <c r="F176" s="2"/>
     </row>
-    <row r="177" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A177" s="2"/>
       <c r="B177" s="2"/>
       <c r="C177" s="2"/>
@@ -2664,7 +2664,7 @@
       <c r="E177" s="2"/>
       <c r="F177" s="2"/>
     </row>
-    <row r="178" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A178" s="2"/>
       <c r="B178" s="2"/>
       <c r="C178" s="2"/>
@@ -2672,7 +2672,7 @@
       <c r="E178" s="2"/>
       <c r="F178" s="2"/>
     </row>
-    <row r="179" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A179" s="2"/>
       <c r="B179" s="2"/>
       <c r="C179" s="2"/>
@@ -2680,7 +2680,7 @@
       <c r="E179" s="2"/>
       <c r="F179" s="2"/>
     </row>
-    <row r="180" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A180" s="2"/>
       <c r="B180" s="2"/>
       <c r="C180" s="2"/>
@@ -2688,7 +2688,7 @@
       <c r="E180" s="2"/>
       <c r="F180" s="2"/>
     </row>
-    <row r="181" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A181" s="2"/>
       <c r="B181" s="2"/>
       <c r="C181" s="2"/>
@@ -2696,7 +2696,7 @@
       <c r="E181" s="2"/>
       <c r="F181" s="2"/>
     </row>
-    <row r="182" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A182" s="2"/>
       <c r="B182" s="2"/>
       <c r="C182" s="2"/>
@@ -2704,7 +2704,7 @@
       <c r="E182" s="2"/>
       <c r="F182" s="2"/>
     </row>
-    <row r="183" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A183" s="2"/>
       <c r="B183" s="2"/>
       <c r="C183" s="2"/>
@@ -2712,7 +2712,7 @@
       <c r="E183" s="2"/>
       <c r="F183" s="2"/>
     </row>
-    <row r="184" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A184" s="2"/>
       <c r="B184" s="2"/>
       <c r="C184" s="2"/>
@@ -2720,7 +2720,7 @@
       <c r="E184" s="2"/>
       <c r="F184" s="2"/>
     </row>
-    <row r="185" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A185" s="2"/>
       <c r="B185" s="2"/>
       <c r="C185" s="2"/>
@@ -2728,7 +2728,7 @@
       <c r="E185" s="2"/>
       <c r="F185" s="2"/>
     </row>
-    <row r="186" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A186" s="2"/>
       <c r="B186" s="2"/>
       <c r="C186" s="2"/>
@@ -2736,7 +2736,7 @@
       <c r="E186" s="2"/>
       <c r="F186" s="2"/>
     </row>
-    <row r="187" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A187" s="2"/>
       <c r="B187" s="2"/>
       <c r="C187" s="2"/>
@@ -2744,7 +2744,7 @@
       <c r="E187" s="2"/>
       <c r="F187" s="2"/>
     </row>
-    <row r="188" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A188" s="2"/>
       <c r="B188" s="2"/>
       <c r="C188" s="2"/>
@@ -2752,7 +2752,7 @@
       <c r="E188" s="2"/>
       <c r="F188" s="2"/>
     </row>
-    <row r="189" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A189" s="2"/>
       <c r="B189" s="2"/>
       <c r="C189" s="2"/>
@@ -2760,7 +2760,7 @@
       <c r="E189" s="2"/>
       <c r="F189" s="2"/>
     </row>
-    <row r="190" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A190" s="2"/>
       <c r="B190" s="2"/>
       <c r="C190" s="2"/>
@@ -2768,7 +2768,7 @@
       <c r="E190" s="2"/>
       <c r="F190" s="2"/>
     </row>
-    <row r="191" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A191" s="2"/>
       <c r="B191" s="2"/>
       <c r="C191" s="2"/>
@@ -2776,7 +2776,7 @@
       <c r="E191" s="2"/>
       <c r="F191" s="2"/>
     </row>
-    <row r="227" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A227" s="2"/>
       <c r="B227" s="2"/>
       <c r="C227" s="2"/>
@@ -2784,7 +2784,7 @@
       <c r="E227" s="2"/>
       <c r="F227" s="2"/>
     </row>
-    <row r="228" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A228" s="2"/>
       <c r="B228" s="2"/>
       <c r="C228" s="2"/>
@@ -2792,7 +2792,7 @@
       <c r="E228" s="2"/>
       <c r="F228" s="2"/>
     </row>
-    <row r="229" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A229" s="2"/>
       <c r="B229" s="2"/>
       <c r="C229" s="2"/>
@@ -2800,7 +2800,7 @@
       <c r="E229" s="2"/>
       <c r="F229" s="2"/>
     </row>
-    <row r="230" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A230" s="2"/>
       <c r="B230" s="2"/>
       <c r="C230" s="2"/>
@@ -2808,7 +2808,7 @@
       <c r="E230" s="2"/>
       <c r="F230" s="2"/>
     </row>
-    <row r="231" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A231" s="2"/>
       <c r="B231" s="2"/>
       <c r="C231" s="2"/>
@@ -2816,7 +2816,7 @@
       <c r="E231" s="2"/>
       <c r="F231" s="2"/>
     </row>
-    <row r="232" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A232" s="2"/>
       <c r="B232" s="2"/>
       <c r="C232" s="2"/>
@@ -2824,7 +2824,7 @@
       <c r="E232" s="2"/>
       <c r="F232" s="2"/>
     </row>
-    <row r="246" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A246" s="2"/>
       <c r="B246" s="2"/>
       <c r="C246" s="2"/>
@@ -2832,7 +2832,7 @@
       <c r="E246" s="2"/>
       <c r="F246" s="2"/>
     </row>
-    <row r="247" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A247" s="2"/>
       <c r="B247" s="2"/>
       <c r="C247" s="2"/>
@@ -2840,7 +2840,7 @@
       <c r="E247" s="2"/>
       <c r="F247" s="2"/>
     </row>
-    <row r="248" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A248" s="2"/>
       <c r="B248" s="2"/>
       <c r="C248" s="2"/>
@@ -2848,7 +2848,7 @@
       <c r="E248" s="2"/>
       <c r="F248" s="2"/>
     </row>
-    <row r="249" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A249" s="2"/>
       <c r="B249" s="2"/>
       <c r="C249" s="2"/>
@@ -2856,7 +2856,7 @@
       <c r="E249" s="2"/>
       <c r="F249" s="2"/>
     </row>
-    <row r="250" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A250" s="2"/>
       <c r="B250" s="2"/>
       <c r="C250" s="2"/>
@@ -2864,7 +2864,7 @@
       <c r="E250" s="2"/>
       <c r="F250" s="2"/>
     </row>
-    <row r="251" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A251" s="2"/>
       <c r="B251" s="2"/>
       <c r="C251" s="2"/>
@@ -2872,7 +2872,7 @@
       <c r="E251" s="2"/>
       <c r="F251" s="2"/>
     </row>
-    <row r="252" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A252" s="2"/>
       <c r="B252" s="2"/>
       <c r="C252" s="2"/>
@@ -2880,7 +2880,7 @@
       <c r="E252" s="2"/>
       <c r="F252" s="2"/>
     </row>
-    <row r="253" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A253" s="2"/>
       <c r="B253" s="2"/>
       <c r="C253" s="2"/>
@@ -2925,7 +2925,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>